<commit_message>
Updated product backlog and focus group document
</commit_message>
<xml_diff>
--- a/Deliverable_2/Blackbear-Consultants_Deliverable_2_ProductBacklog_1.xlsx
+++ b/Deliverable_2/Blackbear-Consultants_Deliverable_2_ProductBacklog_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\Documents\GitHub\Blackbear-Consultants\Deliverable_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Things\Code\COS420\Blackbear-Consultants\Deliverable_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E760234-EC2C-4FDA-9593-F6AA475EF916}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA22BD4-875E-429C-B51B-EBF866B8C200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
     <t>IP</t>
   </si>
   <si>
-    <t>2 &amp; 3</t>
+    <t>2, 3, 4</t>
   </si>
 </sst>
 </file>

</xml_diff>